<commit_message>
Solved some array question form snr sheet
</commit_message>
<xml_diff>
--- a/Snr Sheet.xlsx
+++ b/Snr Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D690255-CE44-417C-8DCE-534B3E5887EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D80C10E-0739-46FA-B5B9-FDB962016405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" firstSheet="17" activeTab="15" xr2:uid="{D5265C2E-6317-3044-9590-C765FDB70368}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1972" uniqueCount="755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1979" uniqueCount="761">
   <si>
     <t>DYNAMIC PROGRAMMING</t>
   </si>
@@ -2334,12 +2334,30 @@
   <si>
     <t>Not Able To Solve In First Attempt</t>
   </si>
+  <si>
+    <t>Subscribe For The Prob</t>
+  </si>
+  <si>
+    <t>Disliked</t>
+  </si>
+  <si>
+    <t>Another way is all num are positive so we can mark them as negative once we found at that index and when we find another one we can conclude its duplicate</t>
+  </si>
+  <si>
+    <t>Diff Approacoh -&gt;</t>
+  </si>
+  <si>
+    <t>Go Through Follow Up (Imp)</t>
+  </si>
+  <si>
+    <t>Follow Up 1-&gt;For This We Store The Prev Row In Buffer And Compare The Current Row With Prev By Shifting Prev Row By One Now If Both Are Same Then We Check For Further  Follow Up 2-&gt;I think the second one, you basically need two file pointer, the first one start at [0][0], the second one starts at [1][1], load two elements each time, compare and move</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2407,8 +2425,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2430,6 +2477,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2499,7 +2564,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -2545,9 +2610,6 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2555,6 +2617,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2964,10 +3053,10 @@
       <c r="T2" s="14"/>
     </row>
     <row r="3" spans="5:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
@@ -3012,16 +3101,16 @@
       <c r="Z4" s="13"/>
     </row>
     <row r="5" spans="5:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
       <c r="O5" s="16"/>
       <c r="P5" s="16"/>
       <c r="Q5" s="16"/>
@@ -3036,18 +3125,18 @@
       <c r="Z5" s="13"/>
     </row>
     <row r="6" spans="5:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
       <c r="S6" s="16"/>
@@ -3060,22 +3149,22 @@
       <c r="Z6" s="13"/>
     </row>
     <row r="7" spans="5:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
       <c r="U7" s="13"/>
       <c r="V7" s="13"/>
       <c r="W7" s="13"/>
@@ -3084,21 +3173,21 @@
       <c r="Z7" s="13"/>
     </row>
     <row r="8" spans="5:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="26"/>
       <c r="T8" s="16"/>
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
@@ -3108,14 +3197,14 @@
       <c r="Z8" s="13"/>
     </row>
     <row r="9" spans="5:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
       <c r="O9" s="16"/>
@@ -3132,22 +3221,22 @@
       <c r="Z9" s="13"/>
     </row>
     <row r="10" spans="5:26" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="26"/>
+      <c r="T10" s="26"/>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
       <c r="W10" s="13"/>
@@ -3180,11 +3269,11 @@
       <c r="Z11" s="13"/>
     </row>
     <row r="12" spans="5:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
@@ -6431,10 +6520,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45438C9-D009-8F4A-BE62-C097380EFD67}">
-  <dimension ref="A2:F109"/>
+  <dimension ref="A2:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6443,10 +6532,11 @@
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="18.125" customWidth="1"/>
     <col min="4" max="4" width="17.875" customWidth="1"/>
-    <col min="5" max="5" width="34.125" customWidth="1"/>
+    <col min="6" max="6" width="35.875" customWidth="1"/>
+    <col min="7" max="7" width="153.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="10" customFormat="1" ht="60.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" s="10" customFormat="1" ht="60.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -6459,11 +6549,8 @@
       <c r="D2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>832</v>
       </c>
@@ -6476,12 +6563,12 @@
       <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" t="s">
+      <c r="E3" s="24" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>905</v>
       </c>
@@ -6494,12 +6581,12 @@
       <c r="D4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" t="s">
+      <c r="E4" s="24" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>950</v>
       </c>
@@ -6512,14 +6599,14 @@
       <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="24" t="s">
+        <v>753</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>754</v>
       </c>
-      <c r="F5" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>561</v>
       </c>
@@ -6532,12 +6619,12 @@
       <c r="D6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="24" t="s">
+        <v>752</v>
+      </c>
+      <c r="F6" s="20"/>
+    </row>
+    <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>1051</v>
       </c>
@@ -6550,12 +6637,12 @@
       <c r="D7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="24" t="s">
+        <v>752</v>
+      </c>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>723</v>
       </c>
@@ -6568,12 +6655,14 @@
       <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" t="s">
+      <c r="E8" s="24" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="21" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>1002</v>
       </c>
@@ -6586,12 +6675,12 @@
       <c r="D9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="24" t="s">
+        <v>752</v>
+      </c>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>969</v>
       </c>
@@ -6604,12 +6693,14 @@
       <c r="D10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" t="s">
+      <c r="E10" s="24" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="22" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>867</v>
       </c>
@@ -6622,12 +6713,12 @@
       <c r="D11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="24" t="s">
+        <v>752</v>
+      </c>
+      <c r="F11" s="23"/>
+    </row>
+    <row r="12" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>442</v>
       </c>
@@ -6640,12 +6731,17 @@
       <c r="D12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="24" t="s">
+        <v>752</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>758</v>
+      </c>
+      <c r="G12" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>766</v>
       </c>
@@ -6658,12 +6754,17 @@
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="19"/>
-      <c r="F13" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="24" t="s">
+        <v>752</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>759</v>
+      </c>
+      <c r="G13" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>280</v>
       </c>
@@ -6676,12 +6777,14 @@
       <c r="D14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="19"/>
-      <c r="F14" t="s">
+      <c r="E14" s="24" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="21" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>1074</v>
       </c>
@@ -6694,12 +6797,12 @@
       <c r="D15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="19"/>
-      <c r="F15" t="s">
+      <c r="E15" s="24" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>695</v>
       </c>
@@ -6712,10 +6815,10 @@
       <c r="D16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" t="s">
-        <v>753</v>
-      </c>
+      <c r="E16" s="24" t="s">
+        <v>752</v>
+      </c>
+      <c r="F16" s="27"/>
     </row>
     <row r="17" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
@@ -6730,10 +6833,10 @@
       <c r="D17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="19"/>
-      <c r="F17" t="s">
-        <v>753</v>
-      </c>
+      <c r="E17" s="24" t="s">
+        <v>752</v>
+      </c>
+      <c r="F17" s="17"/>
     </row>
     <row r="18" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
@@ -6748,9 +6851,11 @@
       <c r="D18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="19"/>
-      <c r="F18" t="s">
+      <c r="E18" s="24" t="s">
         <v>753</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>755</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -6766,10 +6871,10 @@
       <c r="D19" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="F19" t="s">
-        <v>753</v>
-      </c>
+      <c r="E19" s="24" t="s">
+        <v>752</v>
+      </c>
+      <c r="F19" s="17"/>
     </row>
     <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
@@ -6784,10 +6889,10 @@
       <c r="D20" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="19"/>
-      <c r="F20" t="s">
-        <v>753</v>
-      </c>
+      <c r="E20" s="24" t="s">
+        <v>752</v>
+      </c>
+      <c r="F20" s="17"/>
     </row>
     <row r="21" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
@@ -6802,10 +6907,10 @@
       <c r="D21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="19"/>
-      <c r="F21" t="s">
-        <v>753</v>
-      </c>
+      <c r="E21" s="24" t="s">
+        <v>752</v>
+      </c>
+      <c r="F21" s="17"/>
     </row>
     <row r="22" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
@@ -6820,10 +6925,10 @@
       <c r="D22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="19"/>
-      <c r="F22" t="s">
-        <v>753</v>
-      </c>
+      <c r="E22" s="24" t="s">
+        <v>752</v>
+      </c>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
@@ -6838,10 +6943,10 @@
       <c r="D23" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" t="s">
+      <c r="E23" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F23" s="28"/>
     </row>
     <row r="24" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
@@ -6856,10 +6961,10 @@
       <c r="D24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" t="s">
+      <c r="E24" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F24" s="17"/>
     </row>
     <row r="25" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
@@ -6874,10 +6979,10 @@
       <c r="D25" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" t="s">
+      <c r="E25" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F25" s="18"/>
     </row>
     <row r="26" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
@@ -6892,10 +6997,10 @@
       <c r="D26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="19"/>
-      <c r="F26" t="s">
-        <v>753</v>
-      </c>
+      <c r="E26" s="24" t="s">
+        <v>752</v>
+      </c>
+      <c r="F26" s="17"/>
     </row>
     <row r="27" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
@@ -6910,10 +7015,10 @@
       <c r="D27" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="19"/>
-      <c r="F27" t="s">
-        <v>753</v>
-      </c>
+      <c r="E27" s="24" t="s">
+        <v>752</v>
+      </c>
+      <c r="F27" s="17"/>
     </row>
     <row r="28" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
@@ -6928,10 +7033,10 @@
       <c r="D28" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="19"/>
-      <c r="F28" t="s">
+      <c r="E28" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F28" s="18"/>
     </row>
     <row r="29" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
@@ -6946,10 +7051,10 @@
       <c r="D29" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="19"/>
-      <c r="F29" t="s">
+      <c r="E29" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F29" s="18"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
@@ -6964,10 +7069,10 @@
       <c r="D30" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="19"/>
-      <c r="F30" t="s">
+      <c r="E30" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
@@ -6982,10 +7087,10 @@
       <c r="D31" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="19"/>
-      <c r="F31" t="s">
+      <c r="E31" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F31" s="18"/>
     </row>
     <row r="32" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
@@ -7000,10 +7105,10 @@
       <c r="D32" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="19"/>
-      <c r="F32" t="s">
+      <c r="E32" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F32" s="18"/>
     </row>
     <row r="33" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
@@ -7018,10 +7123,10 @@
       <c r="D33" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="19"/>
-      <c r="F33" t="s">
+      <c r="E33" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F33" s="18"/>
     </row>
     <row r="34" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
@@ -7036,10 +7141,10 @@
       <c r="D34" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="19"/>
-      <c r="F34" t="s">
+      <c r="E34" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F34" s="18"/>
     </row>
     <row r="35" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
@@ -7054,10 +7159,10 @@
       <c r="D35" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="19"/>
-      <c r="F35" t="s">
+      <c r="E35" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F35" s="18"/>
     </row>
     <row r="36" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
@@ -7072,10 +7177,10 @@
       <c r="D36" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E36" s="19"/>
-      <c r="F36" t="s">
+      <c r="E36" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F36" s="18"/>
     </row>
     <row r="37" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
@@ -7090,10 +7195,10 @@
       <c r="D37" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E37" s="19"/>
-      <c r="F37" t="s">
+      <c r="E37" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F37" s="18"/>
     </row>
     <row r="38" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
@@ -7108,10 +7213,10 @@
       <c r="D38" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E38" s="19"/>
-      <c r="F38" t="s">
+      <c r="E38" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F38" s="18"/>
     </row>
     <row r="39" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
@@ -7126,10 +7231,10 @@
       <c r="D39" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E39" s="19"/>
-      <c r="F39" t="s">
+      <c r="E39" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F39" s="18"/>
     </row>
     <row r="40" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
@@ -7144,10 +7249,10 @@
       <c r="D40" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E40" s="19"/>
-      <c r="F40" t="s">
+      <c r="E40" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F40" s="18"/>
     </row>
     <row r="41" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
@@ -7162,10 +7267,10 @@
       <c r="D41" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E41" s="19"/>
-      <c r="F41" t="s">
+      <c r="E41" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F41" s="18"/>
     </row>
     <row r="42" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
@@ -7180,10 +7285,10 @@
       <c r="D42" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E42" s="19"/>
-      <c r="F42" t="s">
+      <c r="E42" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F42" s="18"/>
     </row>
     <row r="43" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
@@ -7198,10 +7303,10 @@
       <c r="D43" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E43" s="19"/>
-      <c r="F43" t="s">
+      <c r="E43" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F43" s="18"/>
     </row>
     <row r="44" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
@@ -7216,10 +7321,10 @@
       <c r="D44" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E44" s="19"/>
-      <c r="F44" t="s">
+      <c r="E44" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F44" s="18"/>
     </row>
     <row r="45" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
@@ -7234,10 +7339,10 @@
       <c r="D45" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E45" s="19"/>
-      <c r="F45" t="s">
+      <c r="E45" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F45" s="18"/>
     </row>
     <row r="46" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
@@ -7252,10 +7357,10 @@
       <c r="D46" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E46" s="19"/>
-      <c r="F46" t="s">
+      <c r="E46" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F46" s="18"/>
     </row>
     <row r="47" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
@@ -7270,10 +7375,10 @@
       <c r="D47" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E47" s="19"/>
-      <c r="F47" t="s">
+      <c r="E47" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F47" s="18"/>
     </row>
     <row r="48" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
@@ -7288,10 +7393,10 @@
       <c r="D48" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E48" s="19"/>
-      <c r="F48" t="s">
+      <c r="E48" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F48" s="18"/>
     </row>
     <row r="49" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
@@ -7306,10 +7411,10 @@
       <c r="D49" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E49" s="19"/>
-      <c r="F49" t="s">
+      <c r="E49" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F49" s="18"/>
     </row>
     <row r="50" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
@@ -7324,10 +7429,10 @@
       <c r="D50" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E50" s="19"/>
-      <c r="F50" t="s">
+      <c r="E50" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F50" s="18"/>
     </row>
     <row r="51" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
@@ -7342,10 +7447,10 @@
       <c r="D51" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E51" s="19"/>
-      <c r="F51" t="s">
+      <c r="E51" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F51" s="18"/>
     </row>
     <row r="52" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
@@ -7360,10 +7465,10 @@
       <c r="D52" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E52" s="19"/>
-      <c r="F52" t="s">
+      <c r="E52" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F52" s="18"/>
     </row>
     <row r="53" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
@@ -7378,10 +7483,10 @@
       <c r="D53" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E53" s="19"/>
-      <c r="F53" t="s">
+      <c r="E53" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F53" s="18"/>
     </row>
     <row r="54" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
@@ -7396,10 +7501,10 @@
       <c r="D54" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E54" s="19"/>
-      <c r="F54" t="s">
+      <c r="E54" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F54" s="18"/>
     </row>
     <row r="55" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
@@ -7414,10 +7519,10 @@
       <c r="D55" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E55" s="19"/>
-      <c r="F55" t="s">
+      <c r="E55" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F55" s="18"/>
     </row>
     <row r="56" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
@@ -7432,10 +7537,10 @@
       <c r="D56" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E56" s="19"/>
-      <c r="F56" t="s">
+      <c r="E56" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F56" s="18"/>
     </row>
     <row r="57" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
@@ -7450,10 +7555,10 @@
       <c r="D57" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E57" s="19"/>
-      <c r="F57" t="s">
+      <c r="E57" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F57" s="18"/>
     </row>
     <row r="58" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
@@ -7468,10 +7573,10 @@
       <c r="D58" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E58" s="19"/>
-      <c r="F58" t="s">
+      <c r="E58" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F58" s="18"/>
     </row>
     <row r="59" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
@@ -7486,10 +7591,10 @@
       <c r="D59" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E59" s="19"/>
-      <c r="F59" t="s">
+      <c r="E59" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F59" s="18"/>
     </row>
     <row r="60" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
@@ -7504,10 +7609,10 @@
       <c r="D60" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E60" s="19"/>
-      <c r="F60" t="s">
+      <c r="E60" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F60" s="18"/>
     </row>
     <row r="61" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
@@ -7522,10 +7627,10 @@
       <c r="D61" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E61" s="19"/>
-      <c r="F61" t="s">
+      <c r="E61" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F61" s="18"/>
     </row>
     <row r="62" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
@@ -7540,10 +7645,10 @@
       <c r="D62" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E62" s="19"/>
-      <c r="F62" t="s">
+      <c r="E62" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F62" s="18"/>
     </row>
     <row r="63" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
@@ -7558,10 +7663,10 @@
       <c r="D63" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E63" s="19"/>
-      <c r="F63" t="s">
+      <c r="E63" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F63" s="18"/>
     </row>
     <row r="64" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
@@ -7576,10 +7681,10 @@
       <c r="D64" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E64" s="19"/>
-      <c r="F64" t="s">
+      <c r="E64" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F64" s="18"/>
     </row>
     <row r="65" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
@@ -7594,10 +7699,10 @@
       <c r="D65" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E65" s="19"/>
-      <c r="F65" t="s">
+      <c r="E65" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F65" s="18"/>
     </row>
     <row r="66" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
@@ -7612,10 +7717,10 @@
       <c r="D66" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E66" s="19"/>
-      <c r="F66" t="s">
+      <c r="E66" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F66" s="18"/>
     </row>
     <row r="67" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
@@ -7630,10 +7735,10 @@
       <c r="D67" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E67" s="19"/>
-      <c r="F67" t="s">
+      <c r="E67" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F67" s="18"/>
     </row>
     <row r="68" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
@@ -7648,10 +7753,10 @@
       <c r="D68" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E68" s="19"/>
-      <c r="F68" t="s">
+      <c r="E68" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F68" s="18"/>
     </row>
     <row r="69" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
@@ -7666,10 +7771,10 @@
       <c r="D69" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E69" s="19"/>
-      <c r="F69" t="s">
+      <c r="E69" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F69" s="18"/>
     </row>
     <row r="70" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
@@ -7684,10 +7789,10 @@
       <c r="D70" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E70" s="19"/>
-      <c r="F70" t="s">
+      <c r="E70" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F70" s="18"/>
     </row>
     <row r="71" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
@@ -7702,10 +7807,10 @@
       <c r="D71" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E71" s="19"/>
-      <c r="F71" t="s">
+      <c r="E71" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F71" s="18"/>
     </row>
     <row r="72" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
@@ -7720,10 +7825,10 @@
       <c r="D72" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E72" s="19"/>
-      <c r="F72" t="s">
+      <c r="E72" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F72" s="18"/>
     </row>
     <row r="73" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
@@ -7738,10 +7843,10 @@
       <c r="D73" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E73" s="19"/>
-      <c r="F73" t="s">
+      <c r="E73" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F73" s="18"/>
     </row>
     <row r="74" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
@@ -7756,10 +7861,10 @@
       <c r="D74" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E74" s="19"/>
-      <c r="F74" t="s">
+      <c r="E74" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F74" s="18"/>
     </row>
     <row r="75" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
@@ -7774,10 +7879,10 @@
       <c r="D75" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E75" s="19"/>
-      <c r="F75" t="s">
+      <c r="E75" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F75" s="18"/>
     </row>
     <row r="76" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
@@ -7792,10 +7897,10 @@
       <c r="D76" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E76" s="19"/>
-      <c r="F76" t="s">
+      <c r="E76" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F76" s="18"/>
     </row>
     <row r="77" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
@@ -7810,10 +7915,10 @@
       <c r="D77" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E77" s="19"/>
-      <c r="F77" t="s">
+      <c r="E77" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F77" s="18"/>
     </row>
     <row r="78" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
@@ -7828,10 +7933,10 @@
       <c r="D78" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E78" s="19"/>
-      <c r="F78" t="s">
+      <c r="E78" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F78" s="18"/>
     </row>
     <row r="79" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
@@ -7846,10 +7951,10 @@
       <c r="D79" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E79" s="19"/>
-      <c r="F79" t="s">
+      <c r="E79" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F79" s="18"/>
     </row>
     <row r="80" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
@@ -7864,10 +7969,10 @@
       <c r="D80" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E80" s="19"/>
-      <c r="F80" t="s">
+      <c r="E80" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F80" s="18"/>
     </row>
     <row r="81" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
@@ -7882,10 +7987,10 @@
       <c r="D81" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E81" s="19"/>
-      <c r="F81" t="s">
+      <c r="E81" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F81" s="18"/>
     </row>
     <row r="82" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
@@ -7900,10 +8005,10 @@
       <c r="D82" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E82" s="19"/>
-      <c r="F82" t="s">
+      <c r="E82" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F82" s="18"/>
     </row>
     <row r="83" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
@@ -7918,10 +8023,10 @@
       <c r="D83" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E83" s="19"/>
-      <c r="F83" t="s">
+      <c r="E83" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F83" s="18"/>
     </row>
     <row r="84" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4">
@@ -7936,10 +8041,10 @@
       <c r="D84" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E84" s="19"/>
-      <c r="F84" t="s">
+      <c r="E84" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F84" s="18"/>
     </row>
     <row r="85" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
@@ -7954,10 +8059,10 @@
       <c r="D85" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E85" s="19"/>
-      <c r="F85" t="s">
+      <c r="E85" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F85" s="18"/>
     </row>
     <row r="86" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
@@ -7972,10 +8077,10 @@
       <c r="D86" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E86" s="19"/>
-      <c r="F86" t="s">
+      <c r="E86" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F86" s="18"/>
     </row>
     <row r="87" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
@@ -7990,10 +8095,10 @@
       <c r="D87" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E87" s="19"/>
-      <c r="F87" t="s">
+      <c r="E87" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F87" s="18"/>
     </row>
     <row r="88" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
@@ -8008,10 +8113,10 @@
       <c r="D88" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E88" s="19"/>
-      <c r="F88" t="s">
+      <c r="E88" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F88" s="18"/>
     </row>
     <row r="89" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
@@ -8026,10 +8131,10 @@
       <c r="D89" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E89" s="19"/>
-      <c r="F89" t="s">
+      <c r="E89" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F89" s="18"/>
     </row>
     <row r="90" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
@@ -8044,10 +8149,10 @@
       <c r="D90" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E90" s="19"/>
-      <c r="F90" t="s">
+      <c r="E90" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F90" s="18"/>
     </row>
     <row r="91" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4">
@@ -8062,10 +8167,10 @@
       <c r="D91" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E91" s="19"/>
-      <c r="F91" t="s">
+      <c r="E91" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F91" s="18"/>
     </row>
     <row r="92" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
@@ -8080,10 +8185,10 @@
       <c r="D92" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E92" s="19"/>
-      <c r="F92" t="s">
+      <c r="E92" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F92" s="18"/>
     </row>
     <row r="93" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4">
@@ -8098,10 +8203,10 @@
       <c r="D93" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E93" s="19"/>
-      <c r="F93" t="s">
+      <c r="E93" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F93" s="18"/>
     </row>
     <row r="94" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
@@ -8116,10 +8221,10 @@
       <c r="D94" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E94" s="19"/>
-      <c r="F94" t="s">
+      <c r="E94" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F94" s="18"/>
     </row>
     <row r="95" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4">
@@ -8134,10 +8239,10 @@
       <c r="D95" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E95" s="19"/>
-      <c r="F95" t="s">
+      <c r="E95" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F95" s="18"/>
     </row>
     <row r="96" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
@@ -8152,10 +8257,10 @@
       <c r="D96" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E96" s="19"/>
-      <c r="F96" t="s">
+      <c r="E96" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F96" s="18"/>
     </row>
     <row r="97" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4">
@@ -8170,10 +8275,10 @@
       <c r="D97" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E97" s="19"/>
-      <c r="F97" t="s">
+      <c r="E97" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F97" s="18"/>
     </row>
     <row r="98" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
@@ -8188,10 +8293,10 @@
       <c r="D98" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E98" s="19"/>
-      <c r="F98" t="s">
+      <c r="E98" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F98" s="18"/>
     </row>
     <row r="99" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4">
@@ -8206,10 +8311,10 @@
       <c r="D99" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E99" s="19"/>
-      <c r="F99" t="s">
+      <c r="E99" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F99" s="18"/>
     </row>
     <row r="100" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4">
@@ -8224,10 +8329,10 @@
       <c r="D100" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E100" s="19"/>
-      <c r="F100" t="s">
+      <c r="E100" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F100" s="18"/>
     </row>
     <row r="101" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4">
@@ -8242,10 +8347,10 @@
       <c r="D101" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E101" s="19"/>
-      <c r="F101" t="s">
+      <c r="E101" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F101" s="18"/>
     </row>
     <row r="102" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
@@ -8260,10 +8365,10 @@
       <c r="D102" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E102" s="19"/>
-      <c r="F102" t="s">
+      <c r="E102" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F102" s="18"/>
     </row>
     <row r="103" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4">
@@ -8278,10 +8383,10 @@
       <c r="D103" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E103" s="19"/>
-      <c r="F103" t="s">
+      <c r="E103" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F103" s="18"/>
     </row>
     <row r="104" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
@@ -8296,10 +8401,10 @@
       <c r="D104" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E104" s="19"/>
-      <c r="F104" t="s">
+      <c r="E104" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F104" s="18"/>
     </row>
     <row r="105" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="4">
@@ -8314,10 +8419,10 @@
       <c r="D105" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E105" s="19"/>
-      <c r="F105" t="s">
+      <c r="E105" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F105" s="18"/>
     </row>
     <row r="106" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="4">
@@ -8332,10 +8437,10 @@
       <c r="D106" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E106" s="19"/>
-      <c r="F106" t="s">
+      <c r="E106" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F106" s="18"/>
     </row>
     <row r="107" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="4">
@@ -8350,10 +8455,10 @@
       <c r="D107" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E107" s="19"/>
-      <c r="F107" t="s">
+      <c r="E107" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F107" s="18"/>
     </row>
     <row r="108" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="6">
@@ -8368,16 +8473,16 @@
       <c r="D108" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E108" s="19"/>
-      <c r="F108" t="s">
+      <c r="E108" s="24" t="s">
         <v>753</v>
       </c>
+      <c r="F108" s="18"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E109" s="19"/>
+      <c r="F109" s="18"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E108">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D108">
     <sortCondition descending="1" ref="C1:C108"/>
   </sortState>
   <hyperlinks>
@@ -8489,6 +8594,7 @@
     <hyperlink ref="B28" r:id="rId106" display="https://leetcode.com/problems/array-nesting" xr:uid="{09577079-D346-0D49-8AAE-CF6F904A4BE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId107"/>
 </worksheet>
 </file>
 

</xml_diff>